<commit_message>
fix: update order list
</commit_message>
<xml_diff>
--- a/documentation/order_list_V1.xlsx
+++ b/documentation/order_list_V1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonvalov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonvalov/Documents/mice_task/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C28760A-DE89-FC48-B1B2-4FED9BB036DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B8880E-00F3-E144-9840-BB7BC8D4CF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{8B91018B-20F9-CD43-AEE4-527951079336}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Order List</t>
   </si>
@@ -74,9 +74,6 @@
     <t>B0C8JFZ3D9</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B085MBXWBL?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
-  </si>
-  <si>
     <t>www.amazon.com/dp/B0824VSF74?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
   </si>
   <si>
@@ -120,6 +117,18 @@
   </si>
   <si>
     <t>B0B18QWR3L</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Yibuy-Piece-Gold-Plated-Probes/dp/B07FPFBFV3/ref=pd_sim_hxwPM1_sspa_dk_detail_d_sccl_4_2/139-7520447-8586326?pd_rd_w=Gn7Df&amp;content-id=amzn1.sym.3a852a98-d65f-4301-9bd0-9b589b14d1ef&amp;pf_rd_p=3a852a98-d65f-4301-9bd0-9b589b14d1ef&amp;pf_rd_r=Y2DYMS3YMVP821GA47N1&amp;pd_rd_wg=KgCGL&amp;pd_rd_r=11eb851f-f840-4409-a608-c07e911d9376&amp;pd_rd_i=B07FPFBFV3&amp;psc=1&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWM=</t>
+  </si>
+  <si>
+    <t>https://a.co/d/fCMbUDQ</t>
+  </si>
+  <si>
+    <t>Yibuy 100 Piece Gold Plated PCB Probes Pattern die Part Pin Pogo Pin 1mm Pin</t>
+  </si>
+  <si>
+    <t>B07FPFBFV3</t>
   </si>
 </sst>
 </file>
@@ -742,7 +751,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D19"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +795,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -868,7 +877,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -876,22 +885,22 @@
         <v>1</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="24">
-        <v>9.99</v>
+        <v>7.99</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="K12" s="16"/>
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -899,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -907,14 +916,14 @@
         <v>9.99</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -922,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
@@ -930,14 +939,14 @@
         <v>8.2899999999999991</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="16"/>
       <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -945,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
@@ -953,14 +962,14 @@
         <v>8.69</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -968,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
@@ -976,21 +985,31 @@
         <v>6.99</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="16"/>
       <c r="L16" s="18"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="27"/>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="25">
+        <v>10.99</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>27</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="8"/>
     </row>
@@ -1169,7 +1188,7 @@
       </c>
       <c r="I31" s="29">
         <f>SUM(I10:I30)</f>
-        <v>65.929999999999993</v>
+        <v>74.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add answers to comments
</commit_message>
<xml_diff>
--- a/documentation/order_list_V1.xlsx
+++ b/documentation/order_list_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonvalov/Documents/mice_task/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B8880E-00F3-E144-9840-BB7BC8D4CF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5425E63E-E2DC-4F44-B4B2-FA697CAA0CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{8B91018B-20F9-CD43-AEE4-527951079336}"/>
   </bookViews>
@@ -751,7 +751,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="J17" sqref="J17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>